<commit_message>
figuring out target taxa
</commit_message>
<xml_diff>
--- a/SUMMARY SHEETS/SECPROD_SUMMARY_TOTALS.xlsx
+++ b/SUMMARY SHEETS/SECPROD_SUMMARY_TOTALS.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelleysinning/Library/CloudStorage/GoogleDrive-ksinning@vt.edu/My Drive/Data/saltyC_VirginiaTech/SUMMARY SHEETS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelleysinning/Library/CloudStorage/GoogleDrive-ksinning@vt.edu/My Drive/2023-2025 VT/Data/saltyC_VirginiaTech/SUMMARY SHEETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A45C2E3-101D-6345-BB58-7E1074CF5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BC6321-3C73-A748-AA87-34D3F2BCC9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="26080" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="880" windowWidth="26080" windowHeight="14260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TOTALS" sheetId="1" r:id="rId1"/>
-    <sheet name="TOP FFG for SI" sheetId="4" r:id="rId2"/>
-    <sheet name="FFG" sheetId="2" r:id="rId3"/>
-    <sheet name="SITE SUMMARY" sheetId="3" r:id="rId4"/>
+    <sheet name="TARGET TAXA CORE TOP 5" sheetId="6" r:id="rId1"/>
+    <sheet name="TARGET TAXA CORE BOTTOM 5" sheetId="7" r:id="rId2"/>
+    <sheet name="SI filtered for target taxa" sheetId="9" r:id="rId3"/>
+    <sheet name="TOTALS" sheetId="1" r:id="rId4"/>
+    <sheet name="TOP FFG for SI" sheetId="4" r:id="rId5"/>
+    <sheet name="BOTTOM FFG for SI" sheetId="5" r:id="rId6"/>
+    <sheet name="FFG" sheetId="2" r:id="rId7"/>
+    <sheet name="SITE SUMMARY" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="154">
   <si>
     <t>Genus</t>
   </si>
@@ -432,6 +436,60 @@
   <si>
     <t>Summed Annual Production</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>only in EAS and FRY</t>
+  </si>
+  <si>
+    <t>only in LLC so will have no SI</t>
+  </si>
+  <si>
+    <t>only in RUT so will have no SI</t>
+  </si>
+  <si>
+    <t>No FRY</t>
+  </si>
+  <si>
+    <t>Family and only in FRY</t>
+  </si>
+  <si>
+    <t>only in EAS</t>
+  </si>
+  <si>
+    <t>No EAS</t>
+  </si>
+  <si>
+    <t>Only 4 scrapers that qualify</t>
+  </si>
+  <si>
+    <t>Same as top for scrapers because not enough genera qualify</t>
+  </si>
+  <si>
+    <t>These are all different which I think is cool</t>
+  </si>
+  <si>
+    <t>Taxa</t>
+  </si>
+  <si>
+    <t>wtN</t>
+  </si>
+  <si>
+    <t>wtC</t>
+  </si>
+  <si>
+    <t>Atomic.CN</t>
+  </si>
+  <si>
+    <t>d15N</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>SC.Category</t>
+  </si>
 </sst>
 </file>
 
@@ -440,7 +498,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,13 +540,62 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -514,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,6 +638,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,6 +663,454 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49D54176-8DC6-DC48-8229-FB82929F8A51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6184900" y="609600"/>
+          <a:ext cx="3327400" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>These taxa all occur in EAS, FRY, and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> RIC for production and are the top 5 in production</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39B0378F-ED68-8345-B9EE-C06E3F7F5739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9055100" y="241300"/>
+          <a:ext cx="3327400" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>These taxa all occur in EAS, FRY, and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> RIC for production and are the bottom 5 in production</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Note the scrapers are the same as the top 5 because there are not enough </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AAD1706-6957-1599-FA04-8CA78F0B27D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8902700" y="673100"/>
+          <a:ext cx="3327400" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The target taxa</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> in the previous 2 tabs were filtered with the SI data and unfortunately were not all well represented. Green = in EAS, FRY, and RIC...orange = in 2/3 core sites...unhighlighted = only present in one core site</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>With the SI data we have</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> the only taxa that appear in EAS, FRY, and RIC are Acroneuria, Amphinemura, Hydropsyche, and Pteronarcys</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Amphinemura we know is a tolerant shredder in our top 5 but the rest we haven't focused on</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15070306-A854-1D4E-AD26-DEB07CF347B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="342900"/>
+          <a:ext cx="3327400" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>These taxa DO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> NOT </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>all occur in EAS, FRY, and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> RIC for production so I am disregarding this list</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A67D222D-F08F-2745-A4DE-65B9817416F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6527800" y="342900"/>
+          <a:ext cx="3327400" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>These taxa DO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> NOT </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>all occur in EAS, FRY, and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> RIC for production so I am disregarding this list</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,10 +1399,1175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B115B9-9704-9946-AEF3-FEE71F271470}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.918047473</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.65586213999999998</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.38052138200000002</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="10">
+        <v>8.8141790000000001E-3</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.440221425</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.30746790499999999</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.13406605299999999</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="10">
+        <v>7.3113448999999997E-2</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1.6820681000000001E-2</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="10">
+        <v>23.28552517</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="10">
+        <v>8.7916209869999999</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10">
+        <v>6.7933530009999998</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1.1324433679999999</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.66917991499999996</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E54C31-1B84-BE4F-9843-1710E1D324C0}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10">
+        <v>8.8141790000000001E-3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.38052138200000002</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.65586213999999998</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.918047473</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1.6820681000000001E-2</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="10">
+        <v>7.3113448999999997E-2</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.13406605299999999</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.30746790499999999</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.440221425</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10">
+        <v>7.3981000000000003E-4</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="10">
+        <v>3.1468780000000001E-3</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="10">
+        <v>3.6000630000000001E-3</v>
+      </c>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="10">
+        <v>5.4965300000000003E-3</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="10">
+        <v>9.6403742000000001E-2</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9DE126-8408-4A4E-9083-A4456DC5D3AD}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="10"/>
+      <c r="B1" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="10">
+        <v>5.5533330000000003</v>
+      </c>
+      <c r="D3" s="10">
+        <v>44.003329999999998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>9.5333330000000007</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-0.71666669999999999</v>
+      </c>
+      <c r="G3" s="10">
+        <v>-28.183330000000002</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="10">
+        <v>16</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10.43</v>
+      </c>
+      <c r="D4" s="10">
+        <v>51.42</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5.75</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-32.880000000000003</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="10">
+        <v>16</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="10">
+        <v>7.375</v>
+      </c>
+      <c r="D5" s="10">
+        <v>50.484999999999999</v>
+      </c>
+      <c r="E5" s="10">
+        <v>8.0050000000000008</v>
+      </c>
+      <c r="F5" s="10">
+        <v>-2.2050000000000001</v>
+      </c>
+      <c r="G5" s="10">
+        <v>-27.47</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="10">
+        <v>16</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="10">
+        <v>10.29</v>
+      </c>
+      <c r="D6" s="10">
+        <v>53.19</v>
+      </c>
+      <c r="E6" s="10">
+        <v>6.03</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1.43</v>
+      </c>
+      <c r="G6" s="10">
+        <v>-27.86</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="10">
+        <v>16</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="10">
+        <v>7.5949999999999998</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44.005000000000003</v>
+      </c>
+      <c r="E7" s="10">
+        <v>6.915</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1.76</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-27.625</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="10">
+        <v>16</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="10">
+        <v>12.11</v>
+      </c>
+      <c r="D8" s="10">
+        <v>56.61</v>
+      </c>
+      <c r="E8" s="10">
+        <v>7.06</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.3966666999999999</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-27.63</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="10">
+        <v>16</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10">
+        <v>10.72</v>
+      </c>
+      <c r="D9" s="10">
+        <v>47.25</v>
+      </c>
+      <c r="E9" s="10">
+        <v>5.14</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-26.63</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="10">
+        <v>350</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5.78</v>
+      </c>
+      <c r="D10" s="10">
+        <v>47.56</v>
+      </c>
+      <c r="E10" s="10">
+        <v>9.6</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-1.68</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-28.89</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="10">
+        <v>350</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="10">
+        <v>7.7175000000000002</v>
+      </c>
+      <c r="D11" s="10">
+        <v>47.517499999999998</v>
+      </c>
+      <c r="E11" s="10">
+        <v>7.5374999999999996</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3.1724999999999999</v>
+      </c>
+      <c r="G11" s="10">
+        <v>-25.807500000000001</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="10">
+        <v>350</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="10">
+        <v>8.8825000000000003</v>
+      </c>
+      <c r="D12" s="10">
+        <v>47.427500000000002</v>
+      </c>
+      <c r="E12" s="10">
+        <v>6.2350000000000003</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2.19</v>
+      </c>
+      <c r="G12" s="10">
+        <v>-25.612500000000001</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="10">
+        <v>350</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="D13" s="10">
+        <v>47.2</v>
+      </c>
+      <c r="E13" s="10">
+        <v>5.45</v>
+      </c>
+      <c r="F13" s="10">
+        <v>-0.34</v>
+      </c>
+      <c r="G13" s="10">
+        <v>-30.94</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="10">
+        <v>350</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="10">
+        <v>7.63</v>
+      </c>
+      <c r="D14" s="10">
+        <v>41.35</v>
+      </c>
+      <c r="E14" s="10">
+        <v>8.9</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5.7925000000000004</v>
+      </c>
+      <c r="G14" s="10">
+        <v>-28.377500000000001</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="10">
+        <v>350</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="10">
+        <v>11.29</v>
+      </c>
+      <c r="D15" s="10">
+        <v>49.2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>5.08</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2.88</v>
+      </c>
+      <c r="G15" s="10">
+        <v>-26.09</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="10">
+        <v>350</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="10">
+        <v>8.8550000000000004</v>
+      </c>
+      <c r="D16" s="10">
+        <v>43.82</v>
+      </c>
+      <c r="E16" s="10">
+        <v>5.85</v>
+      </c>
+      <c r="F16" s="10">
+        <v>6.66</v>
+      </c>
+      <c r="G16" s="10">
+        <v>-23.125</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10">
+        <v>10.81</v>
+      </c>
+      <c r="D17" s="10">
+        <v>50.89</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5.49</v>
+      </c>
+      <c r="F17" s="10">
+        <v>4.7</v>
+      </c>
+      <c r="G17" s="10">
+        <v>-24.59</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="10">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10">
+        <v>43.31</v>
+      </c>
+      <c r="E18" s="10">
+        <v>10.11</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="G18" s="10">
+        <v>-28.69</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6.648333</v>
+      </c>
+      <c r="D19" s="10">
+        <v>48.891669999999998</v>
+      </c>
+      <c r="E19" s="10">
+        <v>8.5983330000000002</v>
+      </c>
+      <c r="F19" s="10">
+        <v>7.0883333000000004</v>
+      </c>
+      <c r="G19" s="10">
+        <v>-25.406669999999998</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="10">
+        <v>8.65</v>
+      </c>
+      <c r="D20" s="10">
+        <v>52.74</v>
+      </c>
+      <c r="E20" s="10">
+        <v>7.11</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="G20" s="10">
+        <v>-25.74</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="10">
+        <v>9.2866669999999996</v>
+      </c>
+      <c r="D21" s="10">
+        <v>47.536670000000001</v>
+      </c>
+      <c r="E21" s="10">
+        <v>6.2466670000000004</v>
+      </c>
+      <c r="F21" s="10">
+        <v>5.0033333000000004</v>
+      </c>
+      <c r="G21" s="10">
+        <v>-27.246670000000002</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1185</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G519"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A486" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -12793,12 +14523,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A33C90-033B-5C4D-B01D-3675459FD11C}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12807,7 +14537,7 @@
     <col min="3" max="3" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>122</v>
       </c>
@@ -12817,8 +14547,11 @@
       <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
@@ -12829,7 +14562,7 @@
         <v>0.918047473</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
@@ -12840,7 +14573,7 @@
         <v>0.65586213999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>123</v>
       </c>
@@ -12851,7 +14584,7 @@
         <v>0.38052138200000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>123</v>
       </c>
@@ -12862,18 +14595,21 @@
         <v>8.8141790000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="2">
         <v>2.07872E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>125</v>
       </c>
@@ -12884,7 +14620,7 @@
         <v>0.440221425</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
@@ -12895,7 +14631,7 @@
         <v>0.30746790499999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>125</v>
       </c>
@@ -12906,7 +14642,7 @@
         <v>0.13406605299999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -12917,7 +14653,7 @@
         <v>7.3113448999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>125</v>
       </c>
@@ -12928,7 +14664,7 @@
         <v>1.6820681000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>126</v>
       </c>
@@ -12939,7 +14675,7 @@
         <v>23.28552517</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>126</v>
       </c>
@@ -12950,7 +14686,7 @@
         <v>8.7916209869999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>126</v>
       </c>
@@ -12961,18 +14697,21 @@
         <v>6.7933530009999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="12" t="s">
         <v>115</v>
       </c>
       <c r="C15" s="2">
         <v>2.104234725</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -12985,10 +14724,290 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752D9365-6A36-C84A-A0B9-F72E8B49CB15}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2.8975619999999998E-6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2.07872E-4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="8">
+        <v>8.8141790000000001E-3</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.38052140000000001</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.6558621</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.6820680000000001E-2</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="8">
+        <v>7.3113449999999996E-2</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.13406609999999999</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.30746790000000002</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.44022139999999998</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8">
+        <v>8.6316459999999997E-6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="8">
+        <v>7.9280860000000006E-5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.9499280000000001E-4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.6762399999999998E-4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="8">
+        <v>7.3981000000000003E-4</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="6:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="5"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C275A1-6111-5E45-9F34-48D990D918D8}">
   <dimension ref="A1:E55"/>
   <sheetViews>
@@ -13944,7 +15963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8EA48-78B5-B149-A1BE-1DB6888D6347}">
   <dimension ref="A1:G11"/>
   <sheetViews>

</xml_diff>

<commit_message>
looking at target SI taxa
</commit_message>
<xml_diff>
--- a/SUMMARY SHEETS/SECPROD_SUMMARY_TOTALS.xlsx
+++ b/SUMMARY SHEETS/SECPROD_SUMMARY_TOTALS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelleysinning/Library/CloudStorage/GoogleDrive-ksinning@vt.edu/My Drive/2023-2025 VT/Data/saltyC_VirginiaTech/SUMMARY SHEETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CACFD57-11D7-7448-A2BF-B84AFA17022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60EF19-01FD-4B47-BA20-E6B7B2C21E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="26080" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="720" windowWidth="26080" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI available for top taxa" sheetId="14" r:id="rId1"/>
@@ -523,7 +523,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -655,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,8 +681,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -691,11 +689,11 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -705,6 +703,7 @@
     <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,16 +725,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -750,8 +749,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10896600" y="609600"/>
-          <a:ext cx="2146300" cy="1701800"/>
+          <a:off x="76200" y="4356100"/>
+          <a:ext cx="3365500" cy="1701800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -791,13 +790,28 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> taxa </a:t>
+            <a:t> taxa in production</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>italic = bottom 5 taxa</a:t>
+            <a:t>italic = bottom 5 taxa in production</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>from next 2 tabs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>filterSI.year1 in SI.Year1 code, line 281</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -812,16 +826,112 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7DDD452-E155-BD48-46B6-DBE893501E81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6375400" y="368300"/>
+          <a:ext cx="3327400" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>line 4514 in the 2P3.0 code for all these top target taxa stuff</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -837,7 +947,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6870700" y="609600"/>
-          <a:ext cx="3251200" cy="1498600"/>
+          <a:ext cx="3454400" cy="1701800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -888,7 +998,9 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>taxa different for each stream??</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -897,7 +1009,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -986,7 +1098,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -996,10 +1108,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1015,7 +1127,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8902700" y="673100"/>
-          <a:ext cx="3327400" cy="2133600"/>
+          <a:ext cx="3860800" cy="2781300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1080,6 +1192,11 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>Amphinemura we know is a tolerant shredder in our top 5 but the rest we haven't focused on</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1089,7 +1206,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1177,7 +1294,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1263,6 +1380,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1555,7 +1676,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1596,13 +1717,12 @@
       <c r="K1" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1636,7 +1756,7 @@
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1670,7 +1790,7 @@
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1704,7 +1824,7 @@
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -1738,7 +1858,7 @@
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -1772,7 +1892,7 @@
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1806,7 +1926,7 @@
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -1840,7 +1960,7 @@
       <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1874,7 +1994,7 @@
       <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -1908,7 +2028,7 @@
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="35" t="s">
         <v>100</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1942,7 +2062,7 @@
       <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="35" t="s">
         <v>108</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1976,7 +2096,7 @@
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="39" t="s">
         <v>112</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -2010,7 +2130,7 @@
       <c r="A14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="35" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -2041,13 +2161,13 @@
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D15" s="10">
@@ -2075,13 +2195,13 @@
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="25" t="s">
         <v>125</v>
       </c>
       <c r="D16" s="10">
@@ -2109,13 +2229,13 @@
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D17" s="10">
@@ -2143,13 +2263,13 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D18" s="10">
@@ -2177,13 +2297,13 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D19" s="10">
@@ -2211,13 +2331,13 @@
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D20" s="10">
@@ -2245,13 +2365,13 @@
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D21" s="10">
@@ -3745,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C56EF8-60CC-504A-A1F2-BA3F73D9EB16}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3756,16 +3876,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>135</v>
       </c>
       <c r="E1" s="14" t="s">
@@ -3773,674 +3893,675 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="29">
         <v>1.03936E-4</v>
       </c>
-      <c r="E2" s="30"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="29">
         <v>1.9070459999999999E-3</v>
       </c>
-      <c r="E3" s="29"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>7.7991290000000005E-2</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>0.12617490000000001</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>0.82068920000000001</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>3.6966149999999998E-4</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>7.9441519999999999E-4</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <v>9.7541599999999996E-3</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <v>1.501446E-2</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="29">
         <v>0.13431770000000001</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <v>1.6306319999999999E-6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="29">
         <v>1.9499280000000001E-4</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="29">
         <v>3.9143750000000002E-4</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="29">
         <v>4.9738340000000003E-4</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="29">
         <v>2.5900580000000001E-3</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="31">
         <v>1.03936E-4</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="31">
         <v>5.0321369999999999E-3</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="31">
         <v>3.743192E-2</v>
       </c>
-      <c r="E19" s="29"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="31">
         <v>4.9209009999999997E-2</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="31">
         <v>0.27530250000000001</v>
       </c>
-      <c r="E21" s="29"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="31">
         <v>1.230943E-2</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="31">
         <v>2.6530459999999999E-2</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="31">
         <v>2.8636140000000001E-2</v>
       </c>
-      <c r="E24" s="29"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="31">
         <v>8.1241380000000002E-2</v>
       </c>
-      <c r="E25" s="29"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="31">
         <v>0.11420959999999999</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="27"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="31">
         <v>8.6316459999999997E-6</v>
       </c>
-      <c r="E27" s="29"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="31">
         <v>1.4775839999999999E-5</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="31">
         <v>3.1983180000000001E-5</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="33">
+      <c r="D30" s="31">
         <v>3.4783270000000001E-5</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="31">
         <v>1.3179399999999999E-4</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="30">
         <v>1.407789E-6</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="30">
         <v>4.0653769999999997E-6</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="27"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="30">
         <v>4.5698300000000003E-6</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="30">
         <v>1.1095160000000001E-3</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="30">
         <v>3.8245039999999998E-3</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="30">
         <v>6.0027819999999999E-3</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="30">
         <v>1.9668950000000001E-2</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="30">
         <v>0.17671310000000001</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="27"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="30">
         <v>0.17777390000000001</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D41" s="30">
         <v>2.5146259999999999E-6</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D42" s="30">
         <v>4.5698300000000003E-6</v>
       </c>
-      <c r="E42" s="29"/>
+      <c r="E42" s="27"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D43" s="30">
         <v>1.040913E-5</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="32">
+      <c r="D44" s="30">
         <v>2.1259140000000001E-5</v>
       </c>
-      <c r="E44" s="29"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="32">
+      <c r="D45" s="30">
         <v>6.2234200000000001E-5</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4448,15 +4569,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E7045C-CED6-9348-82E8-F8C016D155D4}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="23" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -4469,7 +4590,7 @@
       <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>135</v>
       </c>
       <c r="E1" s="14" t="s">
@@ -4486,7 +4607,7 @@
       <c r="C2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="24">
         <v>0.82068920000000001</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -4494,19 +4615,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="33">
         <v>0.12617490000000001</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="34" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4520,27 +4641,27 @@
       <c r="C4" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="24">
         <v>7.7991290000000005E-2</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="33">
         <v>1.9070459999999999E-3</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="34" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4554,10 +4675,10 @@
       <c r="C6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>1.03936E-4</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4571,10 +4692,10 @@
       <c r="C7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>0.13431770000000001</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4588,10 +4709,10 @@
       <c r="C8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>1.501446E-2</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4605,10 +4726,10 @@
       <c r="C9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="24">
         <v>9.7541599999999996E-3</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4622,10 +4743,10 @@
       <c r="C10" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>7.9441519999999999E-4</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4639,10 +4760,10 @@
       <c r="C11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="24">
         <v>3.6966149999999998E-4</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4656,10 +4777,10 @@
       <c r="C12" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="24">
         <v>0.147282</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4673,78 +4794,78 @@
       <c r="C13" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="24">
         <v>0.10480200000000001</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="33">
         <v>9.4446199999999994E-2</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="34" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="33">
         <v>8.7288390000000004E-3</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="33">
         <v>6.5550249999999999E-3</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="36">
         <v>0.27530250000000001</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -4756,25 +4877,25 @@
       <c r="C18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="23">
         <v>4.9209009999999997E-2</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="36">
         <v>3.743192E-2</v>
       </c>
-      <c r="E19" s="21"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
@@ -4786,10 +4907,10 @@
       <c r="C20" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="23">
         <v>5.0321369999999999E-3</v>
       </c>
-      <c r="E20" s="21"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
@@ -4801,10 +4922,10 @@
       <c r="C21" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="23">
         <v>1.03936E-4</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
@@ -4816,25 +4937,25 @@
       <c r="C22" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="23">
         <v>0.11420959999999999</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="36">
         <v>8.1241380000000002E-2</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
@@ -4846,10 +4967,10 @@
       <c r="C24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="23">
         <v>2.8636140000000001E-2</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
@@ -4861,10 +4982,10 @@
       <c r="C25" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="23">
         <v>2.6530459999999999E-2</v>
       </c>
-      <c r="E25" s="21"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
@@ -4876,72 +4997,72 @@
       <c r="C26" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="23">
         <v>1.230943E-2</v>
       </c>
-      <c r="E26" s="21"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="36">
         <v>1.4275059999999999</v>
       </c>
-      <c r="E27" s="21"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="36">
         <v>1.229268</v>
       </c>
-      <c r="E28" s="36" t="s">
+      <c r="E28" s="34" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="36">
         <v>0.80902180000000001</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="36">
         <v>0.7556583</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
@@ -4953,231 +5074,231 @@
       <c r="C31" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="23">
         <v>0.45668360000000002</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="19" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="26">
         <v>1.1095160000000001E-3</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="26">
         <v>4.5698300000000003E-6</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="26">
         <v>4.0653769999999997E-6</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="26">
         <v>1.407789E-6</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="26">
         <v>0.17777390000000001</v>
       </c>
-      <c r="E36" s="21"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="26">
         <v>0.17671310000000001</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="26">
         <v>1.9668950000000001E-2</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="40">
+      <c r="D39" s="38">
         <v>6.0027819999999999E-3</v>
       </c>
-      <c r="E39" s="21"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="28">
+      <c r="D40" s="26">
         <v>3.8245039999999998E-3</v>
       </c>
-      <c r="E40" s="21"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="40">
+      <c r="D41" s="38">
         <v>8.7724820000000001</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="40">
+      <c r="D42" s="38">
         <v>4.8134940000000004</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="19"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="40">
+      <c r="D43" s="38">
         <v>0.66129760000000004</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="40">
+      <c r="D44" s="38">
         <v>0.30829060000000003</v>
       </c>
-      <c r="E44" s="21"/>
+      <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="28">
+      <c r="D45" s="26">
         <v>8.727878E-2</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="21"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5189,7 +5310,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5650,31 +5771,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="41" t="s">
         <v>153</v>
       </c>
       <c r="K1" s="10"/>
@@ -5683,15 +5804,15 @@
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>